<commit_message>
Add more finished screen
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <r>
       <rPr>
@@ -188,6 +188,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Difficult</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -228,6 +231,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Khong co screenId</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -304,6 +310,56 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">時間） </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Khong merge cell</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.5.1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">他社受電実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve">時間）</t>
     </r>
   </si>
@@ -311,26 +367,26 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.5.1  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">他社受電実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.6.1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">融通実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -340,7 +396,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
@@ -356,16 +412,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">2.6.1  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">融通実績画面（日報</t>
+      <t xml:space="preserve">2.11.1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">その他実績記録画面（日報</t>
     </r>
     <r>
       <rPr>
@@ -396,16 +452,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">2.11.1  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">その他実績記録画面（日報</t>
+      <t xml:space="preserve">2.12.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">所内電力量実績画面（日報</t>
     </r>
     <r>
       <rPr>
@@ -428,29 +484,32 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.12.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">所内電力量実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
+    <t xml:space="preserve">Hien</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.13.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">特高お客さま負荷実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -460,7 +519,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF000000"/>
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
@@ -468,27 +527,27 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Hien</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.13.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">特高お客さま負荷実績画面（日報</t>
+    <t xml:space="preserve">Chua co screenId</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.15.4  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">水力送電端実績画面（日報</t>
     </r>
     <r>
       <rPr>
@@ -519,16 +578,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">2.15.4  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">水力送電端実績画面（日報</t>
+      <t xml:space="preserve">2.16.1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">火力送電端実績画面（日報</t>
     </r>
     <r>
       <rPr>
@@ -559,16 +618,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">2.16.1  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">火力送電端実績画面（日報</t>
+      <t xml:space="preserve">2.17.1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">新エネ送電端実績画面（日報</t>
     </r>
     <r>
       <rPr>
@@ -599,16 +658,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">2.17.1  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">新エネ送電端実績画面（日報</t>
+      <t xml:space="preserve">2.19.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">気象記録画面（日報</t>
     </r>
     <r>
       <rPr>
@@ -631,24 +690,27 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.19.1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">気象記録画面（日報</t>
+    <t xml:space="preserve">Lay Winpfc4110</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.20.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">水系記録画面（日報</t>
     </r>
     <r>
       <rPr>
@@ -679,16 +741,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">2.20.1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">水系記録画面（日報</t>
+      <t xml:space="preserve">2.21.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">正味自流記録画面（日報</t>
     </r>
     <r>
       <rPr>
@@ -719,16 +781,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">2.21.1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">正味自流記録画面（日報</t>
+      <t xml:space="preserve">2.2.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">溢水電力記録画面（日報</t>
     </r>
     <r>
       <rPr>
@@ -754,26 +816,26 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.2.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">溢水電力記録画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.8.1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">発受電実績画面（県大）（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -783,7 +845,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
@@ -799,16 +861,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">2.8.1  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">発受電実績画面（県大）（日報</t>
+      <t xml:space="preserve">2.9.1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">発受電実績画面（富山東）（日報</t>
     </r>
     <r>
       <rPr>
@@ -834,26 +896,26 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.9.1  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">発受電実績画面（富山東）（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.10.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">発受電実績画面 （富山西）（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -863,37 +925,77 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
         <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.10.2  </t>
-    </r>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">時間１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.10.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">発受電実績画面（富山西）（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">時間２）</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">発受電実績画面 （富山西）（日報</t>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.18.1  </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">エリア送電端実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -907,33 +1009,108 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">時間１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.10.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">発受電実績画面（富山西）（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
+      <t xml:space="preserve">時間） </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">co merge cell</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Winpfc4136</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.1.5   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">水力発電実績画面（月報１） </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(khong merge cell)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.3.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">火力発電実績画面（月報） </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">k merge cell</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.4.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">新エネ発電実績画面（月報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -943,37 +1120,382 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間２）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.18.1  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">エリア送電端実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Winpfc4110</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.5.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">他社受電実績画面（月報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.6.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">融通実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.11.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">その他実績記録画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.12.5  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">所内電力量実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.13.5  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">特高お客さま負荷実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.15.6  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">水力送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.16.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">火力送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.17.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">新エネ送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.2.5  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">溢水電力記録画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Winpfc4110(tham khao)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.8.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">発受電実績画面（県大）（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.9.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">発受電実績画面（富山東）（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.10.4  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">発受電実績画面（富山西）（月報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.10.5  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">発受電実績画面（富山西）（月報２）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.18.2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">エリア送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Giong 2.18.1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.1.8   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">水力発電実績画面（年報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.3.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">火力発電実績画面（年報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.4.4  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">新エネ発電実績画面（年報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -983,89 +1505,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.1.5   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">水力発電実績画面（月報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.3.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">火力発電実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.4.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">新エネ発電実績画面（月報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
@@ -1076,382 +1516,6 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.5.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">他社受電実績画面（月報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.6.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">融通実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.11.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">その他実績記録画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.12.5  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">所内電力量実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.13.5  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">特高お客さま負荷実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.15.6  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">水力送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.16.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">火力送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.17.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">新エネ送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.2.5  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">溢水電力記録画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.8.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">発受電実績画面（県大）（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.9.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">発受電実績画面（富山東）（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.10.4  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">発受電実績画面（富山西）（月報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.10.5  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">発受電実績画面（富山西）（月報２）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.18.2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">エリア送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.1.8   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">水力発電実績画面（年報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.3.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">火力発電実績画面（年報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.4.4  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">新エネ発電実績画面（年報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -1571,7 +1635,17 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">新エネ送電端実績画面（年報）</t>
+      <t xml:space="preserve">新エネ送電端実績画面（年報） </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">khong merge cell</t>
     </r>
   </si>
 </sst>
@@ -1651,7 +1725,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1680,6 +1754,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF70AD47"/>
         <bgColor rgb="FF339966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF00"/>
+        <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -1729,7 +1809,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1766,15 +1846,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1831,7 +1923,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF4472C4"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FF66FF00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF3333"/>
@@ -1855,16 +1947,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.6502057613169"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.38683127572016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.9711934156379"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.38683127572016"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9465020576132"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.38683127572016"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1895,33 +1989,42 @@
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>1</v>
@@ -1929,7 +2032,7 @@
     </row>
     <row r="10" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>3</v>
@@ -1937,55 +2040,67 @@
     </row>
     <row r="11" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
@@ -1993,96 +2108,123 @@
     </row>
     <row r="21" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9" t="s">
-        <v>35</v>
+      <c r="A33" s="12" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9" t="s">
-        <v>36</v>
+      <c r="A34" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>1</v>
@@ -2090,51 +2232,66 @@
     </row>
     <row r="38" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10" t="s">
-        <v>44</v>
+      <c r="A42" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="10" t="s">
-        <v>45</v>
+      <c r="A43" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="11" t="s">
-        <v>46</v>
+      <c r="A44" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="11" t="s">
-        <v>47</v>
+      <c r="A45" s="14" t="s">
+        <v>55</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>1</v>
@@ -2142,27 +2299,36 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tang  lam man hinh 2.1.5
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tang.hoang\Desktop\TODOLIST\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <r>
       <rPr>
@@ -39,30 +43,30 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">発受電実績画面（富山西）（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">30</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">分１）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Phuong</t>
+      <t>発受電実績画面（富山西）（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>分１）</t>
+    </r>
+  </si>
+  <si>
+    <t>Phuong</t>
   </si>
   <si>
     <r>
@@ -82,7 +86,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">発受電実績画面（富山西）（日報</t>
+      <t>発受電実績画面（富山西）（日報</t>
     </r>
     <r>
       <rPr>
@@ -92,7 +96,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">30</t>
+      <t>30</t>
     </r>
     <r>
       <rPr>
@@ -101,11 +105,11 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">分２）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Tang</t>
+      <t>分２）</t>
+    </r>
+  </si>
+  <si>
+    <t>Tang</t>
   </si>
   <si>
     <r>
@@ -125,26 +129,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">エリア送電端実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">30</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">分）</t>
+      <t>エリア送電端実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>分）</t>
     </r>
   </si>
   <si>
@@ -165,30 +169,30 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">水力発電実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Difficult</t>
+      <t>水力発電実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
+    </r>
+  </si>
+  <si>
+    <t>Difficult</t>
   </si>
   <si>
     <r>
@@ -208,30 +212,30 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">停止（溢水）電力集約（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Khong co screenId</t>
+      <t>停止（溢水）電力集約（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
+    </r>
+  </si>
+  <si>
+    <t>Khong co screenId</t>
   </si>
   <si>
     <r>
@@ -251,26 +255,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">火力発電実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
+      <t>火力発電実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
     </r>
   </si>
   <si>
@@ -291,17 +295,17 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">新エネ発電実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
+      <t>新エネ発電実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
     </r>
     <r>
       <rPr>
@@ -320,7 +324,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Khong merge cell</t>
+      <t>Khong merge cell</t>
     </r>
   </si>
   <si>
@@ -341,26 +345,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">他社受電実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
+      <t>他社受電実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
     </r>
   </si>
   <si>
@@ -381,26 +385,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">融通実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
+      <t>融通実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
     </r>
   </si>
   <si>
@@ -421,26 +425,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">その他実績記録画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
+      <t>その他実績記録画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
     </r>
   </si>
   <si>
@@ -461,30 +465,30 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">所内電力量実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Hien</t>
+      <t>所内電力量実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
+    </r>
+  </si>
+  <si>
+    <t>Hien</t>
   </si>
   <si>
     <r>
@@ -504,30 +508,30 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">特高お客さま負荷実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Chua co screenId</t>
+      <t>特高お客さま負荷実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
+    </r>
+  </si>
+  <si>
+    <t>Chua co screenId</t>
   </si>
   <si>
     <r>
@@ -547,26 +551,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">水力送電端実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
+      <t>水力送電端実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
     </r>
   </si>
   <si>
@@ -587,26 +591,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">火力送電端実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
+      <t>火力送電端実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
     </r>
   </si>
   <si>
@@ -627,26 +631,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">新エネ送電端実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
+      <t>新エネ送電端実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
     </r>
   </si>
   <si>
@@ -667,30 +671,30 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">気象記録画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Lay Winpfc4110</t>
+      <t>気象記録画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
+    </r>
+  </si>
+  <si>
+    <t>Lay Winpfc4110</t>
   </si>
   <si>
     <r>
@@ -710,26 +714,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">水系記録画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
+      <t>水系記録画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
     </r>
   </si>
   <si>
@@ -750,26 +754,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">正味自流記録画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
+      <t>正味自流記録画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
     </r>
   </si>
   <si>
@@ -790,26 +794,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">溢水電力記録画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
+      <t>溢水電力記録画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
     </r>
   </si>
   <si>
@@ -830,26 +834,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">発受電実績画面（県大）（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
+      <t>発受電実績画面（県大）（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
     </r>
   </si>
   <si>
@@ -870,26 +874,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">発受電実績画面（富山東）（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間）</t>
+      <t>発受電実績画面（富山東）（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
     </r>
   </si>
   <si>
@@ -910,7 +914,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">発受電実績画面 （富山西）（日報</t>
+      <t>発受電実績画面 （富山西）（日報</t>
     </r>
     <r>
       <rPr>
@@ -920,7 +924,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">1</t>
+      <t>1</t>
     </r>
     <r>
       <rPr>
@@ -929,7 +933,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">時間１）</t>
+      <t>時間１）</t>
     </r>
   </si>
   <si>
@@ -950,26 +954,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">発受電実績画面（富山西）（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間２）</t>
+      <t>発受電実績画面（富山西）（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間２）</t>
     </r>
   </si>
   <si>
@@ -990,7 +994,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">エリア送電端実績画面（日報</t>
+      <t>エリア送電端実績画面（日報</t>
     </r>
     <r>
       <rPr>
@@ -1000,7 +1004,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">1</t>
+      <t>1</t>
     </r>
     <r>
       <rPr>
@@ -1019,11 +1023,11 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">co merge cell</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Winpfc4136</t>
+      <t>co merge cell</t>
+    </r>
+  </si>
+  <si>
+    <t>Winpfc4136</t>
   </si>
   <si>
     <r>
@@ -1053,7 +1057,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(khong merge cell)</t>
+      <t>(khong merge cell)</t>
     </r>
   </si>
   <si>
@@ -1084,7 +1088,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">k merge cell</t>
+      <t>k merge cell</t>
     </r>
   </si>
   <si>
@@ -1105,7 +1109,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">新エネ発電実績画面（月報</t>
+      <t>新エネ発電実績画面（月報</t>
     </r>
     <r>
       <rPr>
@@ -1115,7 +1119,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">1</t>
+      <t>1</t>
     </r>
     <r>
       <rPr>
@@ -1124,11 +1128,11 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Winpfc4110</t>
+      <t>）</t>
+    </r>
+  </si>
+  <si>
+    <t>Winpfc4110</t>
   </si>
   <si>
     <r>
@@ -1148,7 +1152,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">他社受電実績画面（月報１）</t>
+      <t>他社受電実績画面（月報１）</t>
     </r>
   </si>
   <si>
@@ -1169,7 +1173,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">融通実績画面（月報）</t>
+      <t>融通実績画面（月報）</t>
     </r>
   </si>
   <si>
@@ -1190,7 +1194,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">その他実績記録画面（月報）</t>
+      <t>その他実績記録画面（月報）</t>
     </r>
   </si>
   <si>
@@ -1211,7 +1215,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">所内電力量実績画面（月報）</t>
+      <t>所内電力量実績画面（月報）</t>
     </r>
   </si>
   <si>
@@ -1232,7 +1236,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">特高お客さま負荷実績画面（月報）</t>
+      <t>特高お客さま負荷実績画面（月報）</t>
     </r>
   </si>
   <si>
@@ -1253,7 +1257,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">水力送電端実績画面（月報）</t>
+      <t>水力送電端実績画面（月報）</t>
     </r>
   </si>
   <si>
@@ -1274,7 +1278,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">火力送電端実績画面（月報）</t>
+      <t>火力送電端実績画面（月報）</t>
     </r>
   </si>
   <si>
@@ -1295,7 +1299,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">新エネ送電端実績画面（月報）</t>
+      <t>新エネ送電端実績画面（月報）</t>
     </r>
   </si>
   <si>
@@ -1316,11 +1320,11 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">溢水電力記録画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Winpfc4110(tham khao)</t>
+      <t>溢水電力記録画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <t>Winpfc4110(tham khao)</t>
   </si>
   <si>
     <r>
@@ -1340,7 +1344,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">発受電実績画面（県大）（月報）</t>
+      <t>発受電実績画面（県大）（月報）</t>
     </r>
   </si>
   <si>
@@ -1361,7 +1365,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">発受電実績画面（富山東）（月報）</t>
+      <t>発受電実績画面（富山東）（月報）</t>
     </r>
   </si>
   <si>
@@ -1382,7 +1386,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">発受電実績画面（富山西）（月報１）</t>
+      <t>発受電実績画面（富山西）（月報１）</t>
     </r>
   </si>
   <si>
@@ -1403,7 +1407,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">発受電実績画面（富山西）（月報２）</t>
+      <t>発受電実績画面（富山西）（月報２）</t>
     </r>
   </si>
   <si>
@@ -1424,11 +1428,11 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">エリア送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Giong 2.18.1</t>
+      <t>エリア送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <t>Giong 2.18.1</t>
   </si>
   <si>
     <r>
@@ -1448,7 +1452,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">水力発電実績画面（年報１）</t>
+      <t>水力発電実績画面（年報１）</t>
     </r>
   </si>
   <si>
@@ -1469,7 +1473,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">火力発電実績画面（年報）</t>
+      <t>火力発電実績画面（年報）</t>
     </r>
   </si>
   <si>
@@ -1490,26 +1494,26 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">新エネ発電実績画面（年報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">）</t>
+      <t>新エネ発電実績画面（年報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>）</t>
     </r>
   </si>
   <si>
@@ -1530,7 +1534,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">他社受電実績画面（年報１）</t>
+      <t>他社受電実績画面（年報１）</t>
     </r>
   </si>
   <si>
@@ -1551,7 +1555,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">負荷実績画面（年報１）</t>
+      <t>負荷実績画面（年報１）</t>
     </r>
   </si>
   <si>
@@ -1572,7 +1576,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">発受電実績画面（富山西）（年報１）</t>
+      <t>発受電実績画面（富山西）（年報１）</t>
     </r>
   </si>
   <si>
@@ -1593,7 +1597,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">水力送電端実績画面（年報）</t>
+      <t>水力送電端実績画面（年報）</t>
     </r>
   </si>
   <si>
@@ -1614,7 +1618,7 @@
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">火力送電端実績画面（年報）</t>
+      <t>火力送電端実績画面（年報）</t>
     </r>
   </si>
   <si>
@@ -1645,38 +1649,20 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">khong merge cell</t>
+      <t>khong merge cell</t>
     </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="TakaoPGothic"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1776,7 +1762,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1784,101 +1770,57 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1937,31 +1879,306 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.9711934156379"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.38683127572016"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9465020576132"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.38683127572016"/>
+    <col min="1" max="1" width="46"/>
+    <col min="2" max="2" width="9.375"/>
+    <col min="3" max="3" width="12"/>
+    <col min="4" max="4" width="13.875" customWidth="1"/>
+    <col min="5" max="1025" width="9.375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1969,7 +2186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" ht="15">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1977,7 +2194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1985,7 +2202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1993,7 +2210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:3" ht="15">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -2001,7 +2218,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:3" ht="15">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2009,7 +2226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:3" ht="15">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -2017,12 +2234,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:3" ht="15">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2030,7 +2247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:3" ht="15">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -2038,7 +2255,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:3" ht="15">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -2046,7 +2263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:3" ht="15">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -2054,22 +2271,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:3">
       <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:3">
       <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:3">
       <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:3" ht="15">
       <c r="A16" s="4" t="s">
         <v>21</v>
       </c>
@@ -2077,12 +2294,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:4">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:4" ht="15">
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
@@ -2090,7 +2307,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
@@ -2098,7 +2315,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:4" ht="15">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -2106,7 +2323,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:4" ht="15">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -2114,7 +2331,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:4" ht="15">
       <c r="A22" s="7" t="s">
         <v>28</v>
       </c>
@@ -2122,7 +2339,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="39" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:4" ht="15">
       <c r="A23" s="8" t="s">
         <v>29</v>
       </c>
@@ -2130,7 +2347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:4" ht="15">
       <c r="A24" s="9" t="s">
         <v>30</v>
       </c>
@@ -2141,15 +2358,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:4" ht="15">
       <c r="A25" s="10" t="s">
         <v>32</v>
       </c>
+      <c r="B25" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="D25" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:4" ht="15">
       <c r="A26" s="10" t="s">
         <v>33</v>
       </c>
@@ -2157,7 +2377,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:4" ht="15">
       <c r="A27" s="11" t="s">
         <v>34</v>
       </c>
@@ -2168,7 +2388,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:4" ht="15">
       <c r="A28" s="10" t="s">
         <v>36</v>
       </c>
@@ -2176,42 +2396,42 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:3">
       <c r="A33" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:3">
       <c r="A34" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:3" ht="15">
       <c r="A36" s="4" t="s">
         <v>44</v>
       </c>
@@ -2222,7 +2442,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:3" ht="15">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
@@ -2230,7 +2450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:3" ht="15">
       <c r="A38" s="8" t="s">
         <v>47</v>
       </c>
@@ -2238,7 +2458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:3" ht="15">
       <c r="A39" s="8" t="s">
         <v>48</v>
       </c>
@@ -2246,7 +2466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:3" ht="15">
       <c r="A40" s="8" t="s">
         <v>49</v>
       </c>
@@ -2254,7 +2474,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:3" ht="15">
       <c r="A41" s="4" t="s">
         <v>50</v>
       </c>
@@ -2265,7 +2485,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:3" ht="15">
       <c r="A42" s="13" t="s">
         <v>52</v>
       </c>
@@ -2273,7 +2493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:3" ht="15">
       <c r="A43" s="13" t="s">
         <v>53</v>
       </c>
@@ -2281,7 +2501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:3" ht="15">
       <c r="A44" s="14" t="s">
         <v>54</v>
       </c>
@@ -2289,7 +2509,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:3" ht="15">
       <c r="A45" s="14" t="s">
         <v>55</v>
       </c>
@@ -2297,17 +2517,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:3">
       <c r="A46" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:3">
       <c r="A47" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:3" ht="15">
       <c r="A48" s="10" t="s">
         <v>58</v>
       </c>
@@ -2315,7 +2535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:2" ht="15">
       <c r="A49" s="10" t="s">
         <v>59</v>
       </c>
@@ -2323,7 +2543,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:2" ht="15">
       <c r="A50" s="10" t="s">
         <v>60</v>
       </c>
@@ -2332,12 +2552,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pha, Tang added more screen
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tang.hoang\Desktop\TODOLIST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linh.le\Desktop\TODOLIST\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
   <si>
     <r>
       <rPr>
@@ -1033,17 +1033,564 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.4.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>新エネ発電実績画面（月報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>）</t>
+    </r>
+  </si>
+  <si>
+    <t>Winpfc4110</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.5.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>他社受電実績画面（月報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.6.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>融通実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.11.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>その他実績記録画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.12.5  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>所内電力量実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.13.5  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>特高お客さま負荷実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.15.6  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>水力送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.16.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>火力送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.17.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>新エネ送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.2.5  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>溢水電力記録画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <t>Winpfc4110(tham khao)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.8.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（県大）（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.9.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（富山東）（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.10.4  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（富山西）（月報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.10.5  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（富山西）（月報２）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.18.2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>エリア送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <t>Giong 2.18.1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.1.8   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>水力発電実績画面（年報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.3.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>火力発電実績画面（年報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.4.4  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>新エネ発電実績画面（年報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.5.4  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>他社受電実績画面（年報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.7.8  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>負荷実績画面（年報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.10.6  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（富山西）（年報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.16.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>火力送電端実績画面（年報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.17.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">新エネ送電端実績画面（年報） </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>khong merge cell</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.15.8  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>水力送電端実績画面（年報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">2.1.5   </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
@@ -1052,7 +1599,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -1061,20 +1608,16 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
+    <t>Pha</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">2.3.2  </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
@@ -1083,573 +1626,12 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
       <t>k merge cell</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.4.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>新エネ発電実績画面（月報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
-    <t>Winpfc4110</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.5.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>他社受電実績画面（月報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.6.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>融通実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.11.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>その他実績記録画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.12.5  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>所内電力量実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.13.5  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>特高お客さま負荷実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.15.6  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>水力送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.16.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>火力送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.17.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>新エネ送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.2.5  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>溢水電力記録画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <t>Winpfc4110(tham khao)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.8.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（県大）（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.9.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（富山東）（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.10.4  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（富山西）（月報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.10.5  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（富山西）（月報２）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.18.2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>エリア送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <t>Giong 2.18.1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.1.8   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>水力発電実績画面（年報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.3.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>火力発電実績画面（年報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.4.4  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>新エネ発電実績画面（年報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.5.4  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>他社受電実績画面（年報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.7.8  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>負荷実績画面（年報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.10.6  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（富山西）（年報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.15.8  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>水力送電端実績画面（年報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.16.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>火力送電端実績画面（年報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.17.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">新エネ送電端実績画面（年報） </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>khong merge cell</t>
     </r>
   </si>
 </sst>
@@ -1773,7 +1755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1813,6 +1795,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2165,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2359,8 +2344,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="15">
-      <c r="A25" s="10" t="s">
-        <v>32</v>
+      <c r="A25" s="15" t="s">
+        <v>59</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>3</v>
@@ -2370,8 +2355,11 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="15">
-      <c r="A26" s="10" t="s">
-        <v>33</v>
+      <c r="A26" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>22</v>
@@ -2379,18 +2367,18 @@
     </row>
     <row r="27" spans="1:4" ht="15">
       <c r="A27" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15">
       <c r="A28" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>22</v>
@@ -2398,53 +2386,53 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15">
       <c r="A36" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15">
       <c r="A37" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>1</v>
@@ -2452,7 +2440,7 @@
     </row>
     <row r="38" spans="1:3" ht="15">
       <c r="A38" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>3</v>
@@ -2460,7 +2448,7 @@
     </row>
     <row r="39" spans="1:3" ht="15">
       <c r="A39" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>1</v>
@@ -2468,7 +2456,7 @@
     </row>
     <row r="40" spans="1:3" ht="15">
       <c r="A40" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>15</v>
@@ -2476,18 +2464,18 @@
     </row>
     <row r="41" spans="1:3" ht="15">
       <c r="A41" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15">
       <c r="A42" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>3</v>
@@ -2495,7 +2483,7 @@
     </row>
     <row r="43" spans="1:3" ht="15">
       <c r="A43" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>3</v>
@@ -2503,7 +2491,7 @@
     </row>
     <row r="44" spans="1:3" ht="15">
       <c r="A44" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>15</v>
@@ -2511,7 +2499,7 @@
     </row>
     <row r="45" spans="1:3" ht="15">
       <c r="A45" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>1</v>
@@ -2519,12 +2507,12 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15">
@@ -2537,7 +2525,7 @@
     </row>
     <row r="49" spans="1:2" ht="15">
       <c r="A49" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>15</v>
@@ -2545,14 +2533,14 @@
     </row>
     <row r="50" spans="1:2" ht="15">
       <c r="A50" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add more screen(done by Pha)
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
   <si>
     <r>
       <rPr>
@@ -1144,12 +1144,420 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">2.16.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>火力送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.17.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>新エネ送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <t>Winpfc4110(tham khao)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.8.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（県大）（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.9.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（富山東）（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.10.4  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（富山西）（月報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.18.2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>エリア送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <t>Giong 2.18.1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.1.8   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>水力発電実績画面（年報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.3.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>火力発電実績画面（年報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.4.4  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>新エネ発電実績画面（年報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.5.4  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>他社受電実績画面（年報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.7.8  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>負荷実績画面（年報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.10.6  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（富山西）（年報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.16.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>火力送電端実績画面（年報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.15.8  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>水力送電端実績画面（年報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.1.5   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">水力発電実績画面（月報１） </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>(khong merge cell)</t>
+    </r>
+  </si>
+  <si>
+    <t>Pha</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.3.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">火力発電実績画面（月報） </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>k merge cell</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.17.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">新エネ送電端実績画面（年報） </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>khong merge cell</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.13.5  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>特高お客さま負荷実績画面（月報）chua co scren id</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.11.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>その他実績記録画面（月報）easy</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">2.15.6  </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
@@ -1158,61 +1566,12 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.16.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>火力送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.17.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>新エネ送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
       <t xml:space="preserve">2.2.5  </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
@@ -1220,397 +1579,17 @@
     </r>
   </si>
   <si>
-    <t>Winpfc4110(tham khao)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.8.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（県大）（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.9.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（富山東）（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.10.4  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（富山西）（月報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
+    <r>
       <t xml:space="preserve">2.10.5  </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
       <t>発受電実績画面（富山西）（月報２）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.18.2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>エリア送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <t>Giong 2.18.1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.1.8   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>水力発電実績画面（年報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.3.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>火力発電実績画面（年報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.4.4  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>新エネ発電実績画面（年報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.5.4  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>他社受電実績画面（年報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.7.8  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>負荷実績画面（年報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.10.6  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（富山西）（年報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.16.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>火力送電端実績画面（年報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.15.8  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>水力送電端実績画面（年報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.1.5   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">水力発電実績画面（月報１） </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>(khong merge cell)</t>
-    </r>
-  </si>
-  <si>
-    <t>Pha</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.3.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">火力発電実績画面（月報） </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>k merge cell</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.17.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">新エネ送電端実績画面（年報） </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>khong merge cell</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.11.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>その他実績記録画面（月報）easy</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.13.5  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>特高お客さま負荷実績画面（月報）chua co scren id</t>
     </r>
   </si>
 </sst>
@@ -1740,7 +1719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1786,6 +1765,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2138,8 +2123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2333,7 +2318,7 @@
     </row>
     <row r="25" spans="1:4" ht="15">
       <c r="A25" s="15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>3</v>
@@ -2344,10 +2329,10 @@
     </row>
     <row r="26" spans="1:4" ht="15">
       <c r="A26" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>22</v>
@@ -2377,9 +2362,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="16" t="s">
-        <v>60</v>
+    <row r="30" spans="1:4" ht="15">
+      <c r="A30" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2389,38 +2377,41 @@
     </row>
     <row r="32" spans="1:4" ht="25.5">
       <c r="A32" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="12" t="s">
-        <v>37</v>
+      <c r="A33" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15">
+      <c r="A36" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15">
-      <c r="A36" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>1</v>
@@ -2428,7 +2419,7 @@
     </row>
     <row r="38" spans="1:3" ht="15">
       <c r="A38" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>3</v>
@@ -2436,34 +2427,34 @@
     </row>
     <row r="39" spans="1:3" ht="15">
       <c r="A39" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15">
-      <c r="A40" s="8" t="s">
-        <v>45</v>
+      <c r="A40" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15">
       <c r="A41" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15">
       <c r="A42" s="13" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>3</v>
@@ -2471,7 +2462,7 @@
     </row>
     <row r="43" spans="1:3" ht="15">
       <c r="A43" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>3</v>
@@ -2479,7 +2470,7 @@
     </row>
     <row r="44" spans="1:3" ht="15">
       <c r="A44" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>15</v>
@@ -2487,7 +2478,7 @@
     </row>
     <row r="45" spans="1:3" ht="15">
       <c r="A45" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>1</v>
@@ -2495,17 +2486,17 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15">
       <c r="A48" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>1</v>
@@ -2513,7 +2504,7 @@
     </row>
     <row r="49" spans="1:2" ht="15">
       <c r="A49" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>15</v>
@@ -2521,10 +2512,10 @@
     </row>
     <row r="50" spans="1:2" ht="15">
       <c r="A50" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pha add screen 2.19.1
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
   <si>
     <r>
       <rPr>
@@ -654,20 +654,912 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
+    <t>Lay Winpfc4110</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.20.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>水系記録画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.21.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>正味自流記録画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.2.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>溢水電力記録画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.8.1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（県大）（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.9.1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（富山東）（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.10.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面 （富山西）（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.10.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（富山西）（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>時間２）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.18.1  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>エリア送電端実績画面（日報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">時間） </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>co merge cell</t>
+    </r>
+  </si>
+  <si>
+    <t>Winpfc4136</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.4.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>新エネ発電実績画面（月報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>）</t>
+    </r>
+  </si>
+  <si>
+    <t>Winpfc4110</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.5.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>他社受電実績画面（月報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.6.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>融通実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.12.5  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>所内電力量実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.16.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>火力送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.17.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>新エネ送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <t>Winpfc4110(tham khao)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.8.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（県大）（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.9.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（富山東）（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.10.4  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（富山西）（月報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.18.2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>エリア送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <t>Giong 2.18.1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.1.8   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>水力発電実績画面（年報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.3.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>火力発電実績画面（年報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.4.4  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>新エネ発電実績画面（年報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.5.4  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>他社受電実績画面（年報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.7.8  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>負荷実績画面（年報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.10.6  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（富山西）（年報１）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.16.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>火力送電端実績画面（年報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.15.8  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>水力送電端実績画面（年報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.1.5   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">水力発電実績画面（月報１） </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>(khong merge cell)</t>
+    </r>
+  </si>
+  <si>
+    <t>Pha</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.3.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">火力発電実績画面（月報） </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>k merge cell</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.17.3  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">新エネ送電端実績画面（年報） </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>khong merge cell</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.13.5  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>特高お客さま負荷実績画面（月報）chua co scren id</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.11.2  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>その他実績記録画面（月報）easy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.15.6  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>水力送電端実績画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.2.5  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>溢水電力記録画面（月報）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.10.5  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="TakaoPGothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>発受電実績画面（富山西）（月報２）</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">2.19.1 </t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
@@ -676,7 +1568,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
@@ -686,910 +1578,11 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color rgb="FF000000"/>
+        <color rgb="FFFF0000"/>
         <rFont val="TakaoPGothic"/>
         <family val="2"/>
       </rPr>
       <t>時間）</t>
-    </r>
-  </si>
-  <si>
-    <t>Lay Winpfc4110</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.20.1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>水系記録画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>時間）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.21.1 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>正味自流記録画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>時間）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.2.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>溢水電力記録画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>時間）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.8.1  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（県大）（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>時間）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.9.1  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（富山東）（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>時間）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.10.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面 （富山西）（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>時間１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.10.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（富山西）（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>時間２）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.18.1  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>エリア送電端実績画面（日報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">時間） </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>co merge cell</t>
-    </r>
-  </si>
-  <si>
-    <t>Winpfc4136</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.4.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>新エネ発電実績画面（月報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
-    <t>Winpfc4110</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.5.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>他社受電実績画面（月報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.6.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>融通実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.12.5  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>所内電力量実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.16.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>火力送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.17.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>新エネ送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <t>Winpfc4110(tham khao)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.8.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（県大）（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.9.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（富山東）（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.10.4  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（富山西）（月報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.18.2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>エリア送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <t>Giong 2.18.1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.1.8   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>水力発電実績画面（年報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.3.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF3333"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>火力発電実績画面（年報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.4.4  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>新エネ発電実績画面（年報</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.5.4  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>他社受電実績画面（年報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.7.8  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>負荷実績画面（年報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.10.6  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（富山西）（年報１）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.16.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>火力送電端実績画面（年報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.15.8  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>水力送電端実績画面（年報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.1.5   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">水力発電実績画面（月報１） </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>(khong merge cell)</t>
-    </r>
-  </si>
-  <si>
-    <t>Pha</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.3.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">火力発電実績画面（月報） </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>k merge cell</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.17.3  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">新エネ送電端実績画面（年報） </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>khong merge cell</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.13.5  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>特高お客さま負荷実績画面（月報）chua co scren id</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.11.2  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>その他実績記録画面（月報）easy</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.15.6  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>水力送電端実績画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.2.5  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>溢水電力記録画面（月報）</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">2.10.5  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="TakaoPGothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>発受電実績画面（富山西）（月報２）</t>
     </r>
   </si>
 </sst>
@@ -2123,8 +2116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2136,7 +2129,7 @@
     <col min="5" max="1025" width="9.375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2144,7 +2137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -2152,7 +2145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2160,7 +2153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15">
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -2168,7 +2161,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15">
+    <row r="5" spans="1:4" ht="15">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -2176,7 +2169,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15">
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -2184,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15">
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -2192,12 +2185,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15">
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -2205,7 +2198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15">
+    <row r="10" spans="1:4" ht="15">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -2213,7 +2206,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15">
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -2221,7 +2214,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15">
+    <row r="12" spans="1:4" ht="15">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -2229,37 +2222,43 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:4" ht="15">
+      <c r="A16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>22</v>
+      <c r="D16" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15">
       <c r="A18" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>17</v>
@@ -2267,7 +2266,7 @@
     </row>
     <row r="19" spans="1:4" ht="15">
       <c r="A19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>6</v>
@@ -2275,7 +2274,7 @@
     </row>
     <row r="20" spans="1:4" ht="15">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>3</v>
@@ -2283,7 +2282,7 @@
     </row>
     <row r="21" spans="1:4" ht="15">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>15</v>
@@ -2291,7 +2290,7 @@
     </row>
     <row r="22" spans="1:4" ht="15">
       <c r="A22" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>15</v>
@@ -2299,7 +2298,7 @@
     </row>
     <row r="23" spans="1:4" ht="15">
       <c r="A23" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>1</v>
@@ -2307,111 +2306,111 @@
     </row>
     <row r="24" spans="1:4" ht="15">
       <c r="A24" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15">
       <c r="A25" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15">
       <c r="A26" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15">
       <c r="A27" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15">
       <c r="A28" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15">
       <c r="A30" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="25.5">
       <c r="A32" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15">
       <c r="A36" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15">
       <c r="A37" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>1</v>
@@ -2419,7 +2418,7 @@
     </row>
     <row r="38" spans="1:3" ht="15">
       <c r="A38" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>3</v>
@@ -2427,7 +2426,7 @@
     </row>
     <row r="39" spans="1:3" ht="15">
       <c r="A39" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>1</v>
@@ -2435,26 +2434,26 @@
     </row>
     <row r="40" spans="1:3" ht="15">
       <c r="A40" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15">
       <c r="A41" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15">
       <c r="A42" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>3</v>
@@ -2462,7 +2461,7 @@
     </row>
     <row r="43" spans="1:3" ht="15">
       <c r="A43" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>3</v>
@@ -2470,7 +2469,7 @@
     </row>
     <row r="44" spans="1:3" ht="15">
       <c r="A44" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>15</v>
@@ -2478,7 +2477,7 @@
     </row>
     <row r="45" spans="1:3" ht="15">
       <c r="A45" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>1</v>
@@ -2486,17 +2485,17 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15">
       <c r="A48" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>1</v>
@@ -2504,7 +2503,7 @@
     </row>
     <row r="49" spans="1:2" ht="15">
       <c r="A49" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>15</v>
@@ -2512,10 +2511,10 @@
     </row>
     <row r="50" spans="1:2" ht="15">
       <c r="A50" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>